<commit_message>
Book check bug solved
</commit_message>
<xml_diff>
--- a/Book_insert.xlsx
+++ b/Book_insert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LibraryManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83F9D18-BFC0-49EF-B6D6-0DCEBDCB8893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2295A95-20D4-4D86-B386-1AA855D7C93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>300</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>

</xml_diff>